<commit_message>
added wikiimages and conc_time_values to extraction example
</commit_message>
<xml_diff>
--- a/WikiImages/Example1/CvT_data_template_articles_populated_pmid30806398.xlsx
+++ b/WikiImages/Example1/CvT_data_template_articles_populated_pmid30806398.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CGrulke\IdeaProjects\CompTox-PK-CvTdb\WikiImages\Example1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB13A7D7-5E4C-4974-893D-159F802B2714}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A537E26-EA13-4B83-B8AE-A86D1B9C0805}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="4" r:id="rId1"/>
@@ -17623,7 +17623,7 @@
   </sheetPr>
   <dimension ref="A1:R399"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -19451,8 +19451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4392"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19485,289 +19485,505 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.80775444264943896</v>
+      </c>
+      <c r="C2">
+        <v>4.5812807881773399</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3.2310177705977501</v>
+      </c>
+      <c r="C3">
+        <v>3.0295566502462998</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4.4426494345718996</v>
+      </c>
+      <c r="C4">
+        <v>2.2660098522167398</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>9.6930533117931894</v>
+      </c>
+      <c r="C5">
+        <v>1.50246305418719</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>14.9434571890145</v>
+      </c>
+      <c r="C6">
+        <v>1.18226600985221</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>29.886914378029001</v>
+      </c>
+      <c r="C7">
+        <v>0.935960591133005</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>44.830371567043599</v>
+      </c>
+      <c r="C8">
+        <v>0.665024630541871</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>59.773828756058101</v>
+      </c>
+      <c r="C9">
+        <v>0.665024630541871</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>90.064620355411904</v>
+      </c>
+      <c r="C10">
+        <v>0.59113300492610799</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>119.95153473344099</v>
+      </c>
+      <c r="C11">
+        <v>0.59113300492610799</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>179.927302100161</v>
+      </c>
+      <c r="C12">
+        <v>0.60344827586206895</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>240.105008077544</v>
+      </c>
+      <c r="C13">
+        <v>0.40640394088670101</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="4">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1.0006696888522599</v>
+      </c>
+      <c r="C14" s="4">
+        <v>18.043478260869499</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="4">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3.0329177828147502</v>
+      </c>
+      <c r="C15" s="4">
+        <v>11.086956521739101</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="4">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4">
+        <v>5.0956453053094304</v>
+      </c>
+      <c r="C16" s="4">
+        <v>9.2753623188405694</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4">
+        <v>10.109296654990001</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5.5797101449275299</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4">
+        <v>14.844340270622901</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4.85507246376811</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="A19" s="4">
+        <v>2</v>
+      </c>
+      <c r="B19" s="4">
+        <v>29.9406724362936</v>
+      </c>
+      <c r="C19" s="4">
+        <v>3.1159420289855002</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="A20" s="4">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4">
+        <v>44.744230372965099</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1.9565217391304299</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="4">
+        <v>2</v>
+      </c>
+      <c r="B21" s="4">
+        <v>59.850436156329401</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1.88405797101448</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="4">
+        <v>2</v>
+      </c>
+      <c r="B22" s="4">
+        <v>89.767497767703802</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1.88405797101448</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="4">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4">
+        <v>119.68584724225499</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2.10144927536231</v>
+      </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="A24" s="4">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4">
+        <v>179.810598255374</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1.1594202898550601</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="A25" s="4">
+        <v>2</v>
+      </c>
+      <c r="B25" s="4">
+        <v>239.64300432722001</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.86956521739130399</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="A26" s="4">
+        <v>3</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1.1560718455937899</v>
+      </c>
+      <c r="C26" s="4">
+        <v>44.2753623188405</v>
+      </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="4">
+        <v>3</v>
+      </c>
+      <c r="B27" s="4">
+        <v>3.09173020125009</v>
+      </c>
+      <c r="C27" s="4">
+        <v>21.014492753623099</v>
+      </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="A28" s="4">
+        <v>3</v>
+      </c>
+      <c r="B28" s="4">
+        <v>4.8329212171165503</v>
+      </c>
+      <c r="C28" s="4">
+        <v>14.927536231884</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="A29" s="4">
+        <v>3</v>
+      </c>
+      <c r="B29" s="4">
+        <v>9.8397039631842809</v>
+      </c>
+      <c r="C29" s="4">
+        <v>10.072463768115901</v>
+      </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="A30" s="4">
+        <v>3</v>
+      </c>
+      <c r="B30" s="4">
+        <v>14.858936053300299</v>
+      </c>
+      <c r="C30" s="4">
+        <v>7.3188405797101304</v>
+      </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="A31" s="4">
+        <v>3</v>
+      </c>
+      <c r="B31" s="4">
+        <v>29.945394601277499</v>
+      </c>
+      <c r="C31" s="4">
+        <v>3.9130434782608599</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="4">
+        <v>3</v>
+      </c>
+      <c r="B32" s="4">
+        <v>44.897915378803397</v>
+      </c>
+      <c r="C32" s="4">
+        <v>2.8985507246376798</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="A33" s="4">
+        <v>3</v>
+      </c>
+      <c r="B33" s="4">
+        <v>59.852582594958399</v>
+      </c>
+      <c r="C33" s="4">
+        <v>2.2463768115942</v>
+      </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="A34" s="4">
+        <v>3</v>
+      </c>
+      <c r="B34" s="4">
+        <v>90.063706298509501</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1.88405797101448</v>
+      </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="A35" s="4">
+        <v>3</v>
+      </c>
+      <c r="B35" s="4">
+        <v>119.683700803626</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1.7391304347826</v>
+      </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="A36" s="4">
+        <v>3</v>
+      </c>
+      <c r="B36" s="4">
+        <v>180.10938251253501</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1.5942028985507199</v>
+      </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="A37" s="4">
+        <v>3</v>
+      </c>
+      <c r="B37" s="4">
+        <v>239.94479359846099</v>
+      </c>
+      <c r="C37" s="4">
+        <v>1.8115942028985399</v>
+      </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>

</xml_diff>